<commit_message>
rewrite board, piece, pos
</commit_message>
<xml_diff>
--- a/ActionPlan.xlsx
+++ b/ActionPlan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leo\Personal\Projects\lila\li-ja\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leo\Projects\lila\li-ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E718F8A-3D89-4665-96DF-3286F0517D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D21CF5D-D71E-4236-8A85-6E5B35A5FC1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1C291D5E-1E99-48BC-A46C-6EAD5B360DBF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1C291D5E-1E99-48BC-A46C-6EAD5B360DBF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="40">
   <si>
     <t>.gitignore</t>
   </si>
@@ -133,6 +133,27 @@
   </si>
   <si>
     <t>Let's try to manage without method renaming</t>
+  </si>
+  <si>
+    <t>First implementation attempt inspired by Synesso/scala-chess</t>
+  </si>
+  <si>
+    <t>Add credits</t>
+  </si>
+  <si>
+    <t>lila\README.md</t>
+  </si>
+  <si>
+    <t>Use ornicar.scalalib</t>
+  </si>
+  <si>
+    <t>lila\project\Build.scala</t>
+  </si>
+  <si>
+    <t>Partial rewrite of Board, Piece and Pos</t>
+  </si>
+  <si>
+    <t>For now - without Validation, but every function returns a new Board</t>
   </si>
 </sst>
 </file>
@@ -182,11 +203,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,23 +521,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E2963DC-9FBA-42E8-B13F-F42B9BDE156E}">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -525,7 +545,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -533,7 +553,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -541,15 +561,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -557,7 +577,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -565,7 +585,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -573,7 +593,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -581,7 +601,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -589,7 +609,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -597,7 +617,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -605,12 +625,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -618,7 +638,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -626,7 +646,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -634,7 +654,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -642,7 +662,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -650,12 +670,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -663,12 +686,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -679,7 +707,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>21</v>
       </c>
@@ -687,7 +715,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -695,7 +723,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>23</v>
       </c>
@@ -706,7 +734,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -717,7 +745,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>24</v>
       </c>
@@ -728,7 +756,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>25</v>
       </c>
@@ -736,7 +764,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>26</v>
       </c>
@@ -744,7 +772,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>18</v>
       </c>
@@ -755,7 +783,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>27</v>
       </c>
@@ -763,12 +791,86 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>7</v>
       </c>
       <c r="B37" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>35</v>
+      </c>
+      <c r="B41" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>17</v>
+      </c>
+      <c r="B45" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>19</v>
+      </c>
+      <c r="B46" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>37</v>
+      </c>
+      <c r="B47" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>23</v>
+      </c>
+      <c r="B51" t="s">
+        <v>12</v>
+      </c>
+      <c r="C51" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>24</v>
+      </c>
+      <c r="B52" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>26</v>
+      </c>
+      <c r="B53" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rewrite board, fix sonar
</commit_message>
<xml_diff>
--- a/ActionPlan.xlsx
+++ b/ActionPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leo\Projects\lila\li-ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D21CF5D-D71E-4236-8A85-6E5B35A5FC1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7633482-2AB9-4AEF-8467-539D6A0B9350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1C291D5E-1E99-48BC-A46C-6EAD5B360DBF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="41">
   <si>
     <t>.gitignore</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>For now - without Validation, but every function returns a new Board</t>
+  </si>
+  <si>
+    <t>Rewrite board basic functions using validation</t>
   </si>
 </sst>
 </file>
@@ -521,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E2963DC-9FBA-42E8-B13F-F42B9BDE156E}">
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:C57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -873,6 +876,19 @@
         <v>12</v>
       </c>
     </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>23</v>
+      </c>
+      <c r="B57" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
separate game entity and model
</commit_message>
<xml_diff>
--- a/ActionPlan.xlsx
+++ b/ActionPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leo\Projects\lila\li-ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1537289-2CE2-461B-92B5-8E0268899818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{642CCDAE-440E-4A74-9350-A800210FD4AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1C291D5E-1E99-48BC-A46C-6EAD5B360DBF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="43">
   <si>
     <t>.gitignore</t>
   </si>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t>Rewrite Pos</t>
+  </si>
+  <si>
+    <t>Separate mongodb entities and pure chess models</t>
   </si>
 </sst>
 </file>
@@ -527,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E2963DC-9FBA-42E8-B13F-F42B9BDE156E}">
-  <dimension ref="A1:C60"/>
+  <dimension ref="A1:C62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,6 +903,14 @@
         <v>12</v>
       </c>
     </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B62" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
promotion + more visual test
</commit_message>
<xml_diff>
--- a/ActionPlan.xlsx
+++ b/ActionPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leo\Personal\Projects\lila\li-ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D47BA373-5AC9-4853-936E-5FE7365519CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{114449BE-1FE1-476E-9467-47775A1B5628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1C291D5E-1E99-48BC-A46C-6EAD5B360DBF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="53">
   <si>
     <t>.gitignore</t>
   </si>
@@ -190,6 +190,9 @@
   </si>
   <si>
     <t>lila\src\test\scala\model\BoardTest.scala</t>
+  </si>
+  <si>
+    <t>Use play-mini instead of play2</t>
   </si>
 </sst>
 </file>
@@ -567,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E2963DC-9FBA-42E8-B13F-F42B9BDE156E}">
-  <dimension ref="A1:E83"/>
+  <dimension ref="A1:E85"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="C83" sqref="C83"/>
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1061,6 +1064,14 @@
         <v>12</v>
       </c>
     </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B85" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add failing rook tests
</commit_message>
<xml_diff>
--- a/ActionPlan.xlsx
+++ b/ActionPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leo\Personal\Projects\lila\li-ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEDB88AB-414D-4562-B10F-22B3BF272101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEDA7908-549C-49A5-9444-2DDC2AC3F6D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1C291D5E-1E99-48BC-A46C-6EAD5B360DBF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="84">
   <si>
     <t>.gitignore</t>
   </si>
@@ -283,6 +283,9 @@
   </si>
   <si>
     <t>Test and implement Color unary ! operator (!White == Black)</t>
+  </si>
+  <si>
+    <t>Add failing rook tests</t>
   </si>
 </sst>
 </file>
@@ -660,10 +663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E2963DC-9FBA-42E8-B13F-F42B9BDE156E}">
-  <dimension ref="A1:E124"/>
+  <dimension ref="A1:E126"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="C124" sqref="C124"/>
+      <selection activeCell="C126" sqref="C126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1380,6 +1383,14 @@
         <v>12</v>
       </c>
     </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A126" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B126" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
implemented queen and bishop
</commit_message>
<xml_diff>
--- a/ActionPlan.xlsx
+++ b/ActionPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leo\Personal\Projects\lila\li-ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDA4EAC-4493-4364-A5AB-D3E808023547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE5EE3E3-C3EA-45F5-B3A8-0156A2DD789B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1C291D5E-1E99-48BC-A46C-6EAD5B360DBF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="94">
   <si>
     <t>.gitignore</t>
   </si>
@@ -304,6 +304,18 @@
   </si>
   <si>
     <t>Better rook testing</t>
+  </si>
+  <si>
+    <t>Implement directed roles: rook, bishop, queen</t>
+  </si>
+  <si>
+    <t>Implement visual formatting with marked positions</t>
+  </si>
+  <si>
+    <t>Add visual ascii chessboard matcher</t>
+  </si>
+  <si>
+    <t>More position performance pointers</t>
   </si>
 </sst>
 </file>
@@ -681,10 +693,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E2963DC-9FBA-42E8-B13F-F42B9BDE156E}">
-  <dimension ref="A1:E138"/>
+  <dimension ref="A1:E146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
-      <selection activeCell="C138" sqref="C138"/>
+    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
+      <selection activeCell="C146" sqref="C146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1457,6 +1469,32 @@
         <v>12</v>
       </c>
     </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A140" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B140" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A142" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A144" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A146" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B146" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
visual formatting with marked positions
</commit_message>
<xml_diff>
--- a/ActionPlan.xlsx
+++ b/ActionPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leo\Personal\Projects\lila\li-ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE5EE3E3-C3EA-45F5-B3A8-0156A2DD789B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F65163-259A-4357-9509-6B8682E5A01B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1C291D5E-1E99-48BC-A46C-6EAD5B360DBF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="94">
   <si>
     <t>.gitignore</t>
   </si>
@@ -696,7 +696,7 @@
   <dimension ref="A1:E146"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
-      <selection activeCell="C146" sqref="C146"/>
+      <selection activeCell="C142" sqref="C142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1481,6 +1481,9 @@
       <c r="A142" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="B142" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">

</xml_diff>

<commit_message>
visual - small change
</commit_message>
<xml_diff>
--- a/ActionPlan.xlsx
+++ b/ActionPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leo\Personal\Projects\lila\li-ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F65163-259A-4357-9509-6B8682E5A01B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{229C64EC-90CD-4739-87A4-B249E772D13B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1C291D5E-1E99-48BC-A46C-6EAD5B360DBF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="94">
   <si>
     <t>.gitignore</t>
   </si>
@@ -696,7 +696,7 @@
   <dimension ref="A1:E146"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
-      <selection activeCell="C142" sqref="C142"/>
+      <selection activeCell="C144" sqref="C144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1489,6 +1489,9 @@
       <c r="A144" s="1" t="s">
         <v>92</v>
       </c>
+      <c r="B144" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">

</xml_diff>

<commit_message>
knight moves implementation and tests
</commit_message>
<xml_diff>
--- a/ActionPlan.xlsx
+++ b/ActionPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leo\Personal\Projects\lila\li-ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65A994C-B185-4096-AB92-AF27C2802640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86B70CB-B754-497A-B6F3-AA02351CD60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1C291D5E-1E99-48BC-A46C-6EAD5B360DBF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="106">
   <si>
     <t>.gitignore</t>
   </si>
@@ -733,7 +733,7 @@
   <dimension ref="A1:E170"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="C156" sqref="C156"/>
+      <selection activeCell="C158" sqref="C158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1582,6 +1582,9 @@
       <c r="A158" s="1" t="s">
         <v>99</v>
       </c>
+      <c r="B158" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">

</xml_diff>

<commit_message>
extracted Trajectory to separate class
</commit_message>
<xml_diff>
--- a/ActionPlan.xlsx
+++ b/ActionPlan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leo\Personal\Projects\lila\li-ja\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leo\Projects\lila\li-ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86B70CB-B754-497A-B6F3-AA02351CD60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79169791-AE7F-4EB1-8CED-FDDAFE6BEE6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1C291D5E-1E99-48BC-A46C-6EAD5B360DBF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1C291D5E-1E99-48BC-A46C-6EAD5B360DBF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="106">
   <si>
     <t>.gitignore</t>
   </si>
@@ -407,7 +407,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -415,7 +415,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -733,15 +732,15 @@
   <dimension ref="A1:E170"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="C158" sqref="C158"/>
+      <selection activeCell="C162" sqref="C162"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -750,7 +749,7 @@
         <v xml:space="preserve"> installation</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -758,7 +757,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -766,7 +765,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -774,7 +773,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -782,7 +781,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -790,7 +789,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -798,7 +797,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -806,7 +805,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -814,7 +813,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -822,7 +821,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -830,7 +829,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -838,12 +837,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -851,7 +850,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -859,7 +858,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -867,7 +866,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -875,7 +874,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -883,7 +882,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -891,7 +890,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -899,17 +898,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -920,7 +919,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>21</v>
       </c>
@@ -928,7 +927,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -936,7 +935,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>23</v>
       </c>
@@ -947,7 +946,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -958,7 +957,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>24</v>
       </c>
@@ -969,7 +968,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>25</v>
       </c>
@@ -977,7 +976,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>26</v>
       </c>
@@ -985,7 +984,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>18</v>
       </c>
@@ -996,7 +995,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>27</v>
       </c>
@@ -1004,7 +1003,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>7</v>
       </c>
@@ -1012,12 +1011,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>35</v>
       </c>
@@ -1025,12 +1024,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>17</v>
       </c>
@@ -1038,7 +1037,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>19</v>
       </c>
@@ -1046,7 +1045,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>37</v>
       </c>
@@ -1054,12 +1053,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>23</v>
       </c>
@@ -1070,7 +1069,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>24</v>
       </c>
@@ -1078,7 +1077,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>26</v>
       </c>
@@ -1086,12 +1085,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>23</v>
       </c>
@@ -1099,7 +1098,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>41</v>
       </c>
@@ -1107,7 +1106,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>42</v>
       </c>
@@ -1115,7 +1114,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>43</v>
       </c>
@@ -1123,7 +1122,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>44</v>
       </c>
@@ -1131,7 +1130,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>45</v>
       </c>
@@ -1139,7 +1138,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>46</v>
       </c>
@@ -1147,7 +1146,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>47</v>
       </c>
@@ -1155,7 +1154,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>48</v>
       </c>
@@ -1163,12 +1162,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>21</v>
       </c>
@@ -1176,7 +1175,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>22</v>
       </c>
@@ -1184,7 +1183,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>23</v>
       </c>
@@ -1192,7 +1191,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>24</v>
       </c>
@@ -1200,7 +1199,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>50</v>
       </c>
@@ -1208,7 +1207,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>27</v>
       </c>
@@ -1216,7 +1215,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>51</v>
       </c>
@@ -1224,7 +1223,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>52</v>
       </c>
@@ -1232,7 +1231,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>53</v>
       </c>
@@ -1240,7 +1239,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>54</v>
       </c>
@@ -1248,12 +1247,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>56</v>
       </c>
@@ -1261,7 +1260,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>57</v>
       </c>
@@ -1269,7 +1268,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>58</v>
       </c>
@@ -1277,7 +1276,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>59</v>
       </c>
@@ -1285,7 +1284,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>60</v>
       </c>
@@ -1293,7 +1292,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>61</v>
       </c>
@@ -1301,7 +1300,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>62</v>
       </c>
@@ -1309,12 +1308,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>7</v>
       </c>
@@ -1322,7 +1321,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>65</v>
       </c>
@@ -1330,7 +1329,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>66</v>
       </c>
@@ -1338,7 +1337,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>67</v>
       </c>
@@ -1346,7 +1345,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>68</v>
       </c>
@@ -1354,7 +1353,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>59</v>
       </c>
@@ -1362,7 +1361,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>69</v>
       </c>
@@ -1370,7 +1369,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>70</v>
       </c>
@@ -1378,7 +1377,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>61</v>
       </c>
@@ -1386,7 +1385,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>71</v>
       </c>
@@ -1394,7 +1393,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>72</v>
       </c>
@@ -1402,7 +1401,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>76</v>
       </c>
@@ -1410,7 +1409,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>77</v>
       </c>
@@ -1418,7 +1417,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>78</v>
       </c>
@@ -1426,7 +1425,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>79</v>
       </c>
@@ -1434,7 +1433,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>81</v>
       </c>
@@ -1442,7 +1441,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>82</v>
       </c>
@@ -1450,7 +1449,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>83</v>
       </c>
@@ -1458,7 +1457,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>84</v>
       </c>
@@ -1466,7 +1465,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>85</v>
       </c>
@@ -1474,7 +1473,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>86</v>
       </c>
@@ -1482,7 +1481,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>87</v>
       </c>
@@ -1490,7 +1489,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>88</v>
       </c>
@@ -1498,7 +1497,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>89</v>
       </c>
@@ -1506,7 +1505,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>90</v>
       </c>
@@ -1514,7 +1513,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>91</v>
       </c>
@@ -1522,7 +1521,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>92</v>
       </c>
@@ -1530,7 +1529,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>93</v>
       </c>
@@ -1538,7 +1537,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>94</v>
       </c>
@@ -1546,7 +1545,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>95</v>
       </c>
@@ -1554,7 +1553,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>96</v>
       </c>
@@ -1562,7 +1561,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>97</v>
       </c>
@@ -1570,7 +1569,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>98</v>
       </c>
@@ -1578,7 +1577,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>99</v>
       </c>
@@ -1586,35 +1585,38 @@
         <v>12</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B160" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B162" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A169" s="5"/>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>105</v>
       </c>

</xml_diff>

<commit_message>
implement and test basic pawn move
</commit_message>
<xml_diff>
--- a/ActionPlan.xlsx
+++ b/ActionPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leo\Projects\lila\li-ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79169791-AE7F-4EB1-8CED-FDDAFE6BEE6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE2A7BD-1E6F-4782-AA74-C5D3004FF000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1C291D5E-1E99-48BC-A46C-6EAD5B360DBF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="106">
   <si>
     <t>.gitignore</t>
   </si>
@@ -732,7 +732,7 @@
   <dimension ref="A1:E170"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="C162" sqref="C162"/>
+      <selection activeCell="C164" sqref="C164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1605,6 +1605,9 @@
       <c r="A164" s="1" t="s">
         <v>102</v>
       </c>
+      <c r="B164" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">

</xml_diff>

<commit_message>
some utility functions for models
</commit_message>
<xml_diff>
--- a/ActionPlan.xlsx
+++ b/ActionPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leo\Projects\lila\li-ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE2A7BD-1E6F-4782-AA74-C5D3004FF000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B81C78A-88A5-4CA8-BC1C-7D3B860C246E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1C291D5E-1E99-48BC-A46C-6EAD5B360DBF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="106">
   <si>
     <t>.gitignore</t>
   </si>
@@ -732,7 +732,7 @@
   <dimension ref="A1:E170"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="C164" sqref="C164"/>
+      <selection activeCell="C166" sqref="C166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1613,6 +1613,9 @@
       <c r="A166" s="1" t="s">
         <v>103</v>
       </c>
+      <c r="B166" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">

</xml_diff>

<commit_message>
pawn capture and first move
</commit_message>
<xml_diff>
--- a/ActionPlan.xlsx
+++ b/ActionPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leo\Projects\lila\li-ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B81C78A-88A5-4CA8-BC1C-7D3B860C246E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F3D1921-BB8C-4731-B55F-4AB6ABF18415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1C291D5E-1E99-48BC-A46C-6EAD5B360DBF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="106">
   <si>
     <t>.gitignore</t>
   </si>
@@ -732,7 +732,7 @@
   <dimension ref="A1:E170"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="C166" sqref="C166"/>
+      <selection activeCell="C170" sqref="C170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1621,10 +1621,16 @@
       <c r="A168" s="1" t="s">
         <v>104</v>
       </c>
+      <c r="B168" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>105</v>
+      </c>
+      <c r="B170" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pawn 2-square move fix implementation and tests
</commit_message>
<xml_diff>
--- a/ActionPlan.xlsx
+++ b/ActionPlan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leo\Projects\lila\li-ja\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leo\Personal\Projects\lila\li-ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F49AE0A-F5C0-4FE4-B6F0-7E9AA7C6F82D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{888FA233-BE83-4F07-950E-CD51AAACBF4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1C291D5E-1E99-48BC-A46C-6EAD5B360DBF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1C291D5E-1E99-48BC-A46C-6EAD5B360DBF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="126">
   <si>
     <t>.gitignore</t>
   </si>
@@ -793,15 +793,15 @@
   <dimension ref="A1:E208"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
-      <selection activeCell="B170" sqref="B170"/>
+      <selection activeCell="C176" sqref="C176"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="55.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -810,7 +810,7 @@
         <v xml:space="preserve"> installation</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -818,7 +818,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -826,7 +826,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -834,7 +834,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -842,7 +842,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -850,7 +850,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -858,7 +858,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -866,7 +866,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -874,7 +874,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -882,7 +882,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -890,7 +890,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -898,12 +898,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -911,7 +911,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -919,7 +919,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -927,7 +927,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -935,7 +935,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -943,7 +943,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -951,7 +951,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -959,17 +959,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -980,7 +980,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>21</v>
       </c>
@@ -988,7 +988,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -996,7 +996,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>23</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>24</v>
       </c>
@@ -1029,7 +1029,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>25</v>
       </c>
@@ -1037,7 +1037,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>26</v>
       </c>
@@ -1045,7 +1045,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>18</v>
       </c>
@@ -1056,7 +1056,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>27</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>7</v>
       </c>
@@ -1072,12 +1072,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>35</v>
       </c>
@@ -1085,12 +1085,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>17</v>
       </c>
@@ -1098,7 +1098,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>19</v>
       </c>
@@ -1106,7 +1106,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>37</v>
       </c>
@@ -1114,12 +1114,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>23</v>
       </c>
@@ -1130,7 +1130,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>24</v>
       </c>
@@ -1138,7 +1138,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>26</v>
       </c>
@@ -1146,12 +1146,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>23</v>
       </c>
@@ -1159,7 +1159,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>41</v>
       </c>
@@ -1167,7 +1167,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>42</v>
       </c>
@@ -1175,7 +1175,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>43</v>
       </c>
@@ -1183,7 +1183,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
         <v>44</v>
       </c>
@@ -1191,7 +1191,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>45</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>46</v>
       </c>
@@ -1207,7 +1207,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>47</v>
       </c>
@@ -1215,7 +1215,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>48</v>
       </c>
@@ -1223,12 +1223,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>21</v>
       </c>
@@ -1236,7 +1236,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>22</v>
       </c>
@@ -1244,7 +1244,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>23</v>
       </c>
@@ -1252,7 +1252,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>24</v>
       </c>
@@ -1260,7 +1260,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>50</v>
       </c>
@@ -1268,7 +1268,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>27</v>
       </c>
@@ -1276,7 +1276,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>51</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>52</v>
       </c>
@@ -1292,7 +1292,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
         <v>53</v>
       </c>
@@ -1300,7 +1300,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>54</v>
       </c>
@@ -1308,12 +1308,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>56</v>
       </c>
@@ -1321,7 +1321,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>57</v>
       </c>
@@ -1329,7 +1329,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>58</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>59</v>
       </c>
@@ -1345,7 +1345,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>60</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>61</v>
       </c>
@@ -1361,7 +1361,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>62</v>
       </c>
@@ -1369,12 +1369,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>7</v>
       </c>
@@ -1382,7 +1382,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>65</v>
       </c>
@@ -1390,7 +1390,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>66</v>
       </c>
@@ -1398,7 +1398,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>67</v>
       </c>
@@ -1406,7 +1406,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>68</v>
       </c>
@@ -1414,7 +1414,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>59</v>
       </c>
@@ -1422,7 +1422,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>69</v>
       </c>
@@ -1430,7 +1430,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>70</v>
       </c>
@@ -1438,7 +1438,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>61</v>
       </c>
@@ -1446,7 +1446,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>71</v>
       </c>
@@ -1454,7 +1454,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>72</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>76</v>
       </c>
@@ -1470,7 +1470,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>77</v>
       </c>
@@ -1478,7 +1478,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>78</v>
       </c>
@@ -1486,7 +1486,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>79</v>
       </c>
@@ -1494,7 +1494,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>81</v>
       </c>
@@ -1502,7 +1502,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>82</v>
       </c>
@@ -1510,7 +1510,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>83</v>
       </c>
@@ -1518,7 +1518,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>84</v>
       </c>
@@ -1526,7 +1526,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>85</v>
       </c>
@@ -1534,7 +1534,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
         <v>86</v>
       </c>
@@ -1542,7 +1542,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
         <v>87</v>
       </c>
@@ -1550,7 +1550,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
         <v>88</v>
       </c>
@@ -1558,7 +1558,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
         <v>89</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
         <v>90</v>
       </c>
@@ -1574,7 +1574,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
         <v>91</v>
       </c>
@@ -1582,7 +1582,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
         <v>92</v>
       </c>
@@ -1590,7 +1590,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
         <v>93</v>
       </c>
@@ -1598,7 +1598,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
         <v>94</v>
       </c>
@@ -1606,7 +1606,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
         <v>95</v>
       </c>
@@ -1614,7 +1614,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
         <v>96</v>
       </c>
@@ -1622,7 +1622,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
         <v>97</v>
       </c>
@@ -1630,7 +1630,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
         <v>98</v>
       </c>
@@ -1638,7 +1638,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
         <v>99</v>
       </c>
@@ -1646,7 +1646,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
         <v>100</v>
       </c>
@@ -1654,7 +1654,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
         <v>101</v>
       </c>
@@ -1662,7 +1662,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="s">
         <v>102</v>
       </c>
@@ -1670,7 +1670,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="s">
         <v>103</v>
       </c>
@@ -1678,7 +1678,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
         <v>104</v>
       </c>
@@ -1686,7 +1686,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A170" s="1" t="s">
         <v>105</v>
       </c>
@@ -1694,65 +1694,74 @@
         <v>12</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A172" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B172" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A174" s="1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B174" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A176" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B176" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A178" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A180" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A182" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A186" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A188" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A189" s="5"/>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A190" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A192" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A194" s="1" t="s">
         <v>117</v>
       </c>
@@ -1760,37 +1769,37 @@
         <v>118</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A196" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A198" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A200" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A202" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A204" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A206" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A208" s="1" t="s">
         <v>125</v>
       </c>

</xml_diff>

<commit_message>
add actors and refactor tests
</commit_message>
<xml_diff>
--- a/ActionPlan.xlsx
+++ b/ActionPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leo\Personal\Projects\lila\li-ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{888FA233-BE83-4F07-950E-CD51AAACBF4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80EB132D-12B2-4342-BBA2-8F0370B10A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1C291D5E-1E99-48BC-A46C-6EAD5B360DBF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="126">
   <si>
     <t>.gitignore</t>
   </si>
@@ -792,8 +792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E2963DC-9FBA-42E8-B13F-F42B9BDE156E}">
   <dimension ref="A1:E208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
-      <selection activeCell="C176" sqref="C176"/>
+    <sheetView tabSelected="1" topLeftCell="A171" workbookViewId="0">
+      <selection activeCell="C178" sqref="C178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1718,45 +1718,48 @@
         <v>12</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A178" s="1" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B178" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A180" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A182" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A186" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A188" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A189" s="5"/>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A190" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A192" s="1" t="s">
         <v>116</v>
       </c>

</xml_diff>

<commit_message>
history and en passant
</commit_message>
<xml_diff>
--- a/ActionPlan.xlsx
+++ b/ActionPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leo\Personal\Projects\lila\li-ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{483DA3A7-F4EF-4461-9C8A-7173E2723BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C60D7D2-B236-4FE3-BC6A-744D52510125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1C291D5E-1E99-48BC-A46C-6EAD5B360DBF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="126">
   <si>
     <t>.gitignore</t>
   </si>
@@ -793,7 +793,7 @@
   <dimension ref="A1:E208"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A171" workbookViewId="0">
-      <selection activeCell="C180" sqref="C180"/>
+      <selection activeCell="C182" sqref="C182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1738,6 +1738,9 @@
       <c r="A182" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="B182" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">

</xml_diff>

<commit_message>
tests for black pawn en passant
</commit_message>
<xml_diff>
--- a/ActionPlan.xlsx
+++ b/ActionPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leo\Personal\Projects\lila\li-ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C60D7D2-B236-4FE3-BC6A-744D52510125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2794542-F397-4FF9-8B5C-1F8735DBE6ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1C291D5E-1E99-48BC-A46C-6EAD5B360DBF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="126">
   <si>
     <t>.gitignore</t>
   </si>
@@ -793,7 +793,7 @@
   <dimension ref="A1:E208"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A171" workbookViewId="0">
-      <selection activeCell="C182" sqref="C182"/>
+      <selection activeCell="C184" sqref="C184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1746,6 +1746,9 @@
       <c r="A184" s="1" t="s">
         <v>112</v>
       </c>
+      <c r="B184" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A186" s="1" t="s">

</xml_diff>

<commit_message>
import partial board representation
</commit_message>
<xml_diff>
--- a/ActionPlan.xlsx
+++ b/ActionPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leo\Personal\Projects\lila\li-ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D5AD51-27F3-497E-BD0A-C98A5317965E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7380BCF-2BCE-44CB-9C11-9B576298398B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1C291D5E-1E99-48BC-A46C-6EAD5B360DBF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="126">
   <si>
     <t>.gitignore</t>
   </si>
@@ -792,8 +792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E2963DC-9FBA-42E8-B13F-F42B9BDE156E}">
   <dimension ref="A1:E208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A177" workbookViewId="0">
-      <selection activeCell="C186" sqref="C186"/>
+    <sheetView tabSelected="1" topLeftCell="A183" workbookViewId="0">
+      <selection activeCell="C188" sqref="C188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1762,6 +1762,9 @@
       <c r="A188" s="1" t="s">
         <v>114</v>
       </c>
+      <c r="B188" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A189" s="5"/>

</xml_diff>

<commit_message>
add failing king safety tests
</commit_message>
<xml_diff>
--- a/ActionPlan.xlsx
+++ b/ActionPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leo\Personal\Projects\lila\li-ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7380BCF-2BCE-44CB-9C11-9B576298398B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD741A6-7BF0-478C-9D94-CF552E574FB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1C291D5E-1E99-48BC-A46C-6EAD5B360DBF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="126">
   <si>
     <t>.gitignore</t>
   </si>
@@ -793,7 +793,7 @@
   <dimension ref="A1:E208"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A183" workbookViewId="0">
-      <selection activeCell="C188" sqref="C188"/>
+      <selection activeCell="C190" sqref="C190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1773,6 +1773,9 @@
       <c r="A190" s="1" t="s">
         <v>115</v>
       </c>
+      <c r="B190" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A192" s="1" t="s">

</xml_diff>

<commit_message>
more king safety tests
</commit_message>
<xml_diff>
--- a/ActionPlan.xlsx
+++ b/ActionPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leo\Personal\Projects\lila\li-ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD741A6-7BF0-478C-9D94-CF552E574FB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83045F3C-39D2-4EDC-871E-415C9ED90E3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1C291D5E-1E99-48BC-A46C-6EAD5B360DBF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="126">
   <si>
     <t>.gitignore</t>
   </si>
@@ -793,7 +793,7 @@
   <dimension ref="A1:E208"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A183" workbookViewId="0">
-      <selection activeCell="C190" sqref="C190"/>
+      <selection activeCell="B198" sqref="B198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1781,6 +1781,9 @@
       <c r="A192" s="1" t="s">
         <v>116</v>
       </c>
+      <c r="B192" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A194" s="1" t="s">
@@ -1793,6 +1796,9 @@
     <row r="196" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A196" s="1" t="s">
         <v>119</v>
+      </c>
+      <c r="B196" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
king safety - first step
</commit_message>
<xml_diff>
--- a/ActionPlan.xlsx
+++ b/ActionPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leo\Personal\Projects\lila\li-ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83045F3C-39D2-4EDC-871E-415C9ED90E3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB94A33B-72FD-4793-A905-82EA573FC49A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1C291D5E-1E99-48BC-A46C-6EAD5B360DBF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="126">
   <si>
     <t>.gitignore</t>
   </si>
@@ -793,7 +793,7 @@
   <dimension ref="A1:E208"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A183" workbookViewId="0">
-      <selection activeCell="B198" sqref="B198"/>
+      <selection activeCell="C198" sqref="C198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1805,6 +1805,9 @@
       <c r="A198" s="1" t="s">
         <v>120</v>
       </c>
+      <c r="B198" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A200" s="1" t="s">

</xml_diff>

<commit_message>
make safety tests pass
</commit_message>
<xml_diff>
--- a/ActionPlan.xlsx
+++ b/ActionPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leo\Personal\Projects\lila\li-ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB94A33B-72FD-4793-A905-82EA573FC49A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F6EF06F-B1D3-47F3-9BAD-D479DA8A7C32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1C291D5E-1E99-48BC-A46C-6EAD5B360DBF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="126">
   <si>
     <t>.gitignore</t>
   </si>
@@ -793,7 +793,7 @@
   <dimension ref="A1:E208"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A183" workbookViewId="0">
-      <selection activeCell="C198" sqref="C198"/>
+      <selection activeCell="C200" sqref="C200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1813,6 +1813,9 @@
       <c r="A200" s="1" t="s">
         <v>121</v>
       </c>
+      <c r="B200" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A202" s="1" t="s">

</xml_diff>

<commit_message>
check, checkmate and stalemate
</commit_message>
<xml_diff>
--- a/ActionPlan.xlsx
+++ b/ActionPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leo\Projects\lila\li-ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D239C97D-3B1E-4BB6-B127-5EB9BD4C9BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B34B7E-12EC-4B55-BB4F-7237C9640B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1C291D5E-1E99-48BC-A46C-6EAD5B360DBF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="138">
   <si>
     <t>.gitignore</t>
   </si>
@@ -412,6 +412,42 @@
   </si>
   <si>
     <t>Implement check, checkmate and stalemate</t>
+  </si>
+  <si>
+    <t>Introduce Situation class</t>
+  </si>
+  <si>
+    <t>Test check, checkmate and stalemate</t>
+  </si>
+  <si>
+    <t>Add Situation playMoves functions</t>
+  </si>
+  <si>
+    <t>Test complete games</t>
+  </si>
+  <si>
+    <t>Add castle tests</t>
+  </si>
+  <si>
+    <t>Reorganizing moving rules</t>
+  </si>
+  <si>
+    <t>Rename trajectory to longRange</t>
+  </si>
+  <si>
+    <t>Test and implement standard chess kingside castle</t>
+  </si>
+  <si>
+    <t>More castle tests</t>
+  </si>
+  <si>
+    <t>Attempt to generalize castle side</t>
+  </si>
+  <si>
+    <t>Implement and test conditioned pos vectors</t>
+  </si>
+  <si>
+    <t>Remove unused pos functions</t>
   </si>
 </sst>
 </file>
@@ -789,10 +825,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E2963DC-9FBA-42E8-B13F-F42B9BDE156E}">
-  <dimension ref="A1:E208"/>
+  <dimension ref="A1:E232"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A183" workbookViewId="0">
-      <selection activeCell="C206" sqref="C206"/>
+    <sheetView tabSelected="1" topLeftCell="A200" workbookViewId="0">
+      <selection activeCell="B210" sqref="B210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1841,6 +1877,69 @@
       <c r="A208" s="1" t="s">
         <v>125</v>
       </c>
+      <c r="B208" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A210" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A212" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A214" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A216" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A218" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A220" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A222" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A224" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A226" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A228" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A230" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A232" s="1" t="s">
+        <v>137</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
test check, checkmate and stalemate
</commit_message>
<xml_diff>
--- a/ActionPlan.xlsx
+++ b/ActionPlan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leo\Projects\lila\li-ja\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leo\Personal\Projects\lila\li-ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B34B7E-12EC-4B55-BB4F-7237C9640B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4006409-75A4-4791-B55E-89F07F934027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1C291D5E-1E99-48BC-A46C-6EAD5B360DBF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1C291D5E-1E99-48BC-A46C-6EAD5B360DBF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="138">
   <si>
     <t>.gitignore</t>
   </si>
@@ -828,15 +828,15 @@
   <dimension ref="A1:E232"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A200" workbookViewId="0">
-      <selection activeCell="B210" sqref="B210"/>
+      <selection activeCell="C212" sqref="C212"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="55.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -845,7 +845,7 @@
         <v xml:space="preserve"> installation</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -853,7 +853,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -861,7 +861,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -869,7 +869,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -877,7 +877,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -885,7 +885,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -893,7 +893,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -901,7 +901,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -909,7 +909,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -917,7 +917,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -925,7 +925,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -933,12 +933,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -946,7 +946,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -954,7 +954,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -962,7 +962,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -970,7 +970,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -978,7 +978,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -986,7 +986,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -994,17 +994,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>21</v>
       </c>
@@ -1023,7 +1023,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>23</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -1053,7 +1053,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>24</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>25</v>
       </c>
@@ -1072,7 +1072,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>26</v>
       </c>
@@ -1080,7 +1080,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>18</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>27</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>7</v>
       </c>
@@ -1107,12 +1107,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>35</v>
       </c>
@@ -1120,12 +1120,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>17</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>19</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>37</v>
       </c>
@@ -1149,12 +1149,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>23</v>
       </c>
@@ -1165,7 +1165,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>24</v>
       </c>
@@ -1173,7 +1173,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>26</v>
       </c>
@@ -1181,12 +1181,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>23</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>41</v>
       </c>
@@ -1202,7 +1202,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>42</v>
       </c>
@@ -1210,7 +1210,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>43</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
         <v>44</v>
       </c>
@@ -1226,7 +1226,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>45</v>
       </c>
@@ -1234,7 +1234,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>46</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>47</v>
       </c>
@@ -1250,7 +1250,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>48</v>
       </c>
@@ -1258,12 +1258,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>21</v>
       </c>
@@ -1271,7 +1271,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>22</v>
       </c>
@@ -1279,7 +1279,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>23</v>
       </c>
@@ -1287,7 +1287,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>24</v>
       </c>
@@ -1295,7 +1295,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>50</v>
       </c>
@@ -1303,7 +1303,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>27</v>
       </c>
@@ -1311,7 +1311,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>51</v>
       </c>
@@ -1319,7 +1319,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>52</v>
       </c>
@@ -1327,7 +1327,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
         <v>53</v>
       </c>
@@ -1335,7 +1335,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>54</v>
       </c>
@@ -1343,12 +1343,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>56</v>
       </c>
@@ -1356,7 +1356,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>57</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>58</v>
       </c>
@@ -1372,7 +1372,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>59</v>
       </c>
@@ -1380,7 +1380,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>60</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>61</v>
       </c>
@@ -1396,7 +1396,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>62</v>
       </c>
@@ -1404,12 +1404,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>7</v>
       </c>
@@ -1417,7 +1417,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>65</v>
       </c>
@@ -1425,7 +1425,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>66</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>67</v>
       </c>
@@ -1441,7 +1441,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>68</v>
       </c>
@@ -1449,7 +1449,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>59</v>
       </c>
@@ -1457,7 +1457,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>69</v>
       </c>
@@ -1465,7 +1465,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>70</v>
       </c>
@@ -1473,7 +1473,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>61</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>71</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>72</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>76</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>77</v>
       </c>
@@ -1513,7 +1513,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>78</v>
       </c>
@@ -1521,7 +1521,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>79</v>
       </c>
@@ -1529,7 +1529,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>81</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>82</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>83</v>
       </c>
@@ -1553,7 +1553,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>84</v>
       </c>
@@ -1561,7 +1561,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>85</v>
       </c>
@@ -1569,7 +1569,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
         <v>86</v>
       </c>
@@ -1577,7 +1577,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
         <v>87</v>
       </c>
@@ -1585,7 +1585,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
         <v>88</v>
       </c>
@@ -1593,7 +1593,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
         <v>89</v>
       </c>
@@ -1601,7 +1601,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
         <v>90</v>
       </c>
@@ -1609,7 +1609,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
         <v>91</v>
       </c>
@@ -1617,7 +1617,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
         <v>92</v>
       </c>
@@ -1625,7 +1625,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
         <v>93</v>
       </c>
@@ -1633,7 +1633,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
         <v>94</v>
       </c>
@@ -1641,7 +1641,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
         <v>95</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
         <v>96</v>
       </c>
@@ -1657,7 +1657,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
         <v>97</v>
       </c>
@@ -1665,7 +1665,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
         <v>98</v>
       </c>
@@ -1673,7 +1673,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
         <v>99</v>
       </c>
@@ -1681,7 +1681,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
         <v>100</v>
       </c>
@@ -1689,7 +1689,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
         <v>101</v>
       </c>
@@ -1697,7 +1697,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="s">
         <v>102</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="s">
         <v>103</v>
       </c>
@@ -1713,7 +1713,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
         <v>104</v>
       </c>
@@ -1721,7 +1721,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A170" s="1" t="s">
         <v>105</v>
       </c>
@@ -1729,7 +1729,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A172" s="1" t="s">
         <v>106</v>
       </c>
@@ -1737,7 +1737,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A174" s="1" t="s">
         <v>107</v>
       </c>
@@ -1745,7 +1745,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A176" s="1" t="s">
         <v>108</v>
       </c>
@@ -1753,7 +1753,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A178" s="1" t="s">
         <v>109</v>
       </c>
@@ -1761,7 +1761,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A180" s="1" t="s">
         <v>110</v>
       </c>
@@ -1769,7 +1769,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A182" s="1" t="s">
         <v>111</v>
       </c>
@@ -1777,7 +1777,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
         <v>112</v>
       </c>
@@ -1785,7 +1785,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A186" s="1" t="s">
         <v>113</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A188" s="1" t="s">
         <v>114</v>
       </c>
@@ -1801,7 +1801,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A190" s="1" t="s">
         <v>115</v>
       </c>
@@ -1809,7 +1809,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A192" s="1" t="s">
         <v>116</v>
       </c>
@@ -1817,7 +1817,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A194" s="1" t="s">
         <v>117</v>
       </c>
@@ -1825,7 +1825,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A196" s="1" t="s">
         <v>119</v>
       </c>
@@ -1833,7 +1833,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A198" s="1" t="s">
         <v>120</v>
       </c>
@@ -1841,7 +1841,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A200" s="1" t="s">
         <v>121</v>
       </c>
@@ -1849,7 +1849,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A202" s="1" t="s">
         <v>122</v>
       </c>
@@ -1857,7 +1857,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A204" s="1" t="s">
         <v>123</v>
       </c>
@@ -1865,7 +1865,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A206" s="1" t="s">
         <v>124</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A208" s="1" t="s">
         <v>125</v>
       </c>
@@ -1881,62 +1881,68 @@
         <v>12</v>
       </c>
     </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A210" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B210" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A212" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B212" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A214" s="3" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A216" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A218" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A220" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A222" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A224" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A226" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A228" s="1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A230" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A232" s="1" t="s">
         <v>137</v>
       </c>

</xml_diff>

<commit_message>
renamed trajectory to longRange
</commit_message>
<xml_diff>
--- a/ActionPlan.xlsx
+++ b/ActionPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leo\Personal\Projects\lila\li-ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{764DB64B-195E-43F7-A00F-D8B2DA074797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA8A31B-5C5C-46BD-B4CC-942A3837D274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1C291D5E-1E99-48BC-A46C-6EAD5B360DBF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="138">
   <si>
     <t>.gitignore</t>
   </si>
@@ -828,7 +828,7 @@
   <dimension ref="A1:E232"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A215" workbookViewId="0">
-      <selection activeCell="C220" sqref="C220"/>
+      <selection activeCell="C222" sqref="C222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1933,6 +1933,9 @@
       <c r="A222" s="1" t="s">
         <v>132</v>
       </c>
+      <c r="B222" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A224" s="1" t="s">

</xml_diff>

<commit_message>
implement standard chess castle kingside
</commit_message>
<xml_diff>
--- a/ActionPlan.xlsx
+++ b/ActionPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leo\Personal\Projects\lila\li-ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA8A31B-5C5C-46BD-B4CC-942A3837D274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B19C69-303A-49E1-893D-9C928F2149F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1C291D5E-1E99-48BC-A46C-6EAD5B360DBF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="138">
   <si>
     <t>.gitignore</t>
   </si>
@@ -828,7 +828,7 @@
   <dimension ref="A1:E232"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A215" workbookViewId="0">
-      <selection activeCell="C222" sqref="C222"/>
+      <selection activeCell="C224" sqref="C224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1941,6 +1941,9 @@
       <c r="A224" s="1" t="s">
         <v>133</v>
       </c>
+      <c r="B224" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A226" s="1" t="s">

</xml_diff>

<commit_message>
attempt to generalize castle side
</commit_message>
<xml_diff>
--- a/ActionPlan.xlsx
+++ b/ActionPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leo\Personal\Projects\lila\li-ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4631F74F-F22E-463A-8557-37B371833E39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10556A3B-20C2-430D-856C-C6EFBA30FE32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1C291D5E-1E99-48BC-A46C-6EAD5B360DBF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="138">
   <si>
     <t>.gitignore</t>
   </si>
@@ -828,7 +828,7 @@
   <dimension ref="A1:E232"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A215" workbookViewId="0">
-      <selection activeCell="C226" sqref="C226"/>
+      <selection activeCell="C228" sqref="C228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1957,6 +1957,9 @@
       <c r="A228" s="1" t="s">
         <v>135</v>
       </c>
+      <c r="B228" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A230" s="1" t="s">

</xml_diff>

<commit_message>
remove unused pos functions
</commit_message>
<xml_diff>
--- a/ActionPlan.xlsx
+++ b/ActionPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leo\Personal\Projects\lila\li-ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC8C278-266E-430B-A4BB-E7DE9BA54870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{709117A1-036D-44CE-9DE1-8C8051AC8482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1C291D5E-1E99-48BC-A46C-6EAD5B360DBF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="160">
   <si>
     <t>.gitignore</t>
   </si>
@@ -153,9 +153,6 @@
     <t>Partial rewrite of Board, Piece and Pos</t>
   </si>
   <si>
-    <t>For now - without Validation, but every function returns a new Board</t>
-  </si>
-  <si>
     <t>Rewrite board basic functions using validation</t>
   </si>
   <si>
@@ -448,6 +445,75 @@
   </si>
   <si>
     <t>Remove unused pos functions</t>
+  </si>
+  <si>
+    <t>Better history and castling implementation</t>
+  </si>
+  <si>
+    <t>Fix KingTest</t>
+  </si>
+  <si>
+    <t>New history allows castles</t>
+  </si>
+  <si>
+    <t>Improve Board.taking performance (one copy instead of two)</t>
+  </si>
+  <si>
+    <t>Castling or moving rook prevent further castles</t>
+  </si>
+  <si>
+    <t>Move the king prevents castles</t>
+  </si>
+  <si>
+    <t>Small perf improvement</t>
+  </si>
+  <si>
+    <t>Castle under threat tests</t>
+  </si>
+  <si>
+    <t>Don't castle if the enemy threatens part of the king trip</t>
+  </si>
+  <si>
+    <t>Implications optimizations</t>
+  </si>
+  <si>
+    <t>Reorganize code in subproject, add the http and benchmark projects</t>
+  </si>
+  <si>
+    <t>Add google caliper jar</t>
+  </si>
+  <si>
+    <t>Complete game benchmarks</t>
+  </si>
+  <si>
+    <t>Custom travis build script</t>
+  </si>
+  <si>
+    <t>Move chess tests to package lila.chess</t>
+  </si>
+  <si>
+    <t>Remove all chess dependencies</t>
+  </si>
+  <si>
+    <t>Remove Role.longRange</t>
+  </si>
+  <si>
+    <t>Add promotion tests</t>
+  </si>
+  <si>
+    <t>Implement promotion with user choice</t>
+  </si>
+  <si>
+    <t>Refactor to introduce Move</t>
+  </si>
+  <si>
+    <t>Remove model namespace</t>
+  </si>
+  <si>
+    <t>Remove unused imports</t>
+  </si>
+  <si>
+    <t>Start refactoring the test suite</t>
   </si>
 </sst>
 </file>
@@ -503,7 +569,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -511,6 +577,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -825,21 +892,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E2963DC-9FBA-42E8-B13F-F42B9BDE156E}">
-  <dimension ref="A1:E232"/>
+  <dimension ref="A1:E280"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A215" workbookViewId="0">
-      <selection activeCell="C230" sqref="C230"/>
+    <sheetView tabSelected="1" topLeftCell="A222" workbookViewId="0">
+      <selection activeCell="B234" sqref="B234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="55.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="C1" s="5">
+        <v>40958</v>
+      </c>
       <c r="E1" s="4" t="str">
         <f>RIGHT(A1, LEN(A1)-35)</f>
         <v xml:space="preserve"> installation</v>
@@ -937,6 +1008,9 @@
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="C15" s="5">
+        <v>40958</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -946,7 +1020,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -954,7 +1028,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -962,7 +1036,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -970,7 +1044,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -978,7 +1052,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -986,7 +1060,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -994,28 +1068,31 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C25" s="5">
+        <v>40960</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>15</v>
       </c>
       <c r="B27" t="s">
         <v>12</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>21</v>
       </c>
@@ -1023,7 +1100,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -1031,40 +1108,40 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>23</v>
       </c>
       <c r="B30" t="s">
         <v>13</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>16</v>
       </c>
       <c r="B31" t="s">
         <v>12</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>24</v>
       </c>
       <c r="B32" t="s">
         <v>13</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>25</v>
       </c>
@@ -1072,7 +1149,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>26</v>
       </c>
@@ -1080,18 +1157,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>18</v>
       </c>
       <c r="B35" t="s">
         <v>13</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>27</v>
       </c>
@@ -1099,7 +1176,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>7</v>
       </c>
@@ -1107,12 +1184,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C40" s="5">
+        <v>40960</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>35</v>
       </c>
@@ -1120,12 +1200,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C44" s="5">
+        <v>40960</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>17</v>
       </c>
@@ -1133,7 +1216,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>19</v>
       </c>
@@ -1141,7 +1224,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>37</v>
       </c>
@@ -1153,6 +1236,9 @@
       <c r="A50" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="C50" s="5">
+        <v>40960</v>
+      </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
@@ -1161,9 +1247,6 @@
       <c r="B51" t="s">
         <v>12</v>
       </c>
-      <c r="C51" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
@@ -1183,7 +1266,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
+      </c>
+      <c r="C56" s="5">
+        <v>40960</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
@@ -1196,74 +1282,101 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B60" t="s">
         <v>12</v>
+      </c>
+      <c r="C60" s="5">
+        <v>40960</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B62" t="s">
         <v>12</v>
+      </c>
+      <c r="C62" s="5">
+        <v>40960</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B64" t="s">
+        <v>12</v>
+      </c>
+      <c r="C64" s="5">
+        <v>40960</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B64" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" s="3" t="s">
+      <c r="B66" t="s">
+        <v>12</v>
+      </c>
+      <c r="C66" s="5">
+        <v>40960</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B66" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A68" s="1" t="s">
+      <c r="B68" t="s">
+        <v>12</v>
+      </c>
+      <c r="C68" s="5">
+        <v>40960</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B68" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A70" s="1" t="s">
+      <c r="B70" t="s">
+        <v>12</v>
+      </c>
+      <c r="C70" s="5">
+        <v>40960</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B70" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A72" s="1" t="s">
+      <c r="B72" t="s">
+        <v>12</v>
+      </c>
+      <c r="C72" s="5">
+        <v>40960</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B72" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A74" s="1" t="s">
+      <c r="B74" t="s">
+        <v>12</v>
+      </c>
+      <c r="C74" s="5">
+        <v>40960</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B74" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A76" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C76" s="5">
+        <v>40960</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>21</v>
       </c>
@@ -1271,7 +1384,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>22</v>
       </c>
@@ -1279,7 +1392,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>23</v>
       </c>
@@ -1287,7 +1400,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>24</v>
       </c>
@@ -1295,15 +1408,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B81" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>27</v>
       </c>
@@ -1311,105 +1424,123 @@
         <v>12</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
+        <v>50</v>
+      </c>
+      <c r="B83" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B83" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A85" s="1" t="s">
+      <c r="B85" t="s">
+        <v>12</v>
+      </c>
+      <c r="C85" s="5">
+        <v>40962</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="B85" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A87" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="B87" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C87" s="5">
+        <v>40962</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B89" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C89" s="5">
+        <v>40962</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C91" s="5">
+        <v>40962</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
-        <v>56</v>
       </c>
       <c r="B92" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
+        <v>56</v>
+      </c>
+      <c r="B93" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
         <v>57</v>
       </c>
-      <c r="B93" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
+      <c r="B94" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
         <v>58</v>
       </c>
-      <c r="B94" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
+      <c r="B95" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
         <v>59</v>
       </c>
-      <c r="B95" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
+      <c r="B96" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
         <v>60</v>
       </c>
-      <c r="B96" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
+      <c r="B97" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B97" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A99" s="1" t="s">
+      <c r="B99" t="s">
         <v>62</v>
       </c>
-      <c r="B99" t="s">
+      <c r="C99" s="5">
+        <v>40962</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A101" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A101" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C101" s="5">
+        <v>40962</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>7</v>
       </c>
@@ -1417,562 +1548,932 @@
         <v>13</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
+        <v>64</v>
+      </c>
+      <c r="B103" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
         <v>65</v>
       </c>
-      <c r="B103" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A104" t="s">
+      <c r="B104" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
         <v>66</v>
       </c>
-      <c r="B104" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
+      <c r="B105" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
         <v>67</v>
       </c>
-      <c r="B105" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A106" t="s">
+      <c r="B106" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>58</v>
+      </c>
+      <c r="B107" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
         <v>68</v>
       </c>
-      <c r="B106" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
-        <v>59</v>
-      </c>
-      <c r="B107" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A108" t="s">
+      <c r="B108" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
         <v>69</v>
-      </c>
-      <c r="B108" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A109" t="s">
-        <v>70</v>
       </c>
       <c r="B109" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B110" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>70</v>
+      </c>
+      <c r="B111" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>71</v>
+      </c>
+      <c r="B112" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A114" s="1" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A111" t="s">
-        <v>71</v>
-      </c>
-      <c r="B111" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A112" t="s">
-        <v>72</v>
-      </c>
-      <c r="B112" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A114" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="B114" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C114" s="5">
+        <v>40962</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B116" t="s">
+        <v>12</v>
+      </c>
+      <c r="C116" s="5">
+        <v>40962</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A118" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B116" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A118" s="1" t="s">
+      <c r="B118" t="s">
+        <v>12</v>
+      </c>
+      <c r="C118" s="5">
+        <v>40962</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A120" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B118" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A120" s="1" t="s">
+      <c r="B120" t="s">
         <v>79</v>
       </c>
-      <c r="B120" t="s">
+      <c r="C120" s="5">
+        <v>40962</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A122" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A122" s="1" t="s">
+      <c r="B122" t="s">
+        <v>12</v>
+      </c>
+      <c r="C122" s="5">
+        <v>40962</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A124" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B122" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A124" s="1" t="s">
+      <c r="B124" t="s">
+        <v>12</v>
+      </c>
+      <c r="C124" s="5">
+        <v>40962</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A126" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B124" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A126" s="1" t="s">
+      <c r="B126" t="s">
+        <v>12</v>
+      </c>
+      <c r="C126" s="5">
+        <v>40962</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A128" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="B126" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A128" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="B128" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C128" s="5">
+        <v>40962</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B130" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C130" s="5">
+        <v>40962</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B132" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C132" s="5">
+        <v>40962</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B134" t="s">
+        <v>62</v>
+      </c>
+      <c r="C134" s="5">
+        <v>40962</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A136" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B134" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A136" s="1" t="s">
+      <c r="B136" t="s">
+        <v>12</v>
+      </c>
+      <c r="C136" s="5">
+        <v>40962</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A138" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B136" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A138" s="1" t="s">
+      <c r="B138" t="s">
+        <v>12</v>
+      </c>
+      <c r="C138" s="5">
+        <v>40962</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A140" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B138" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A140" s="1" t="s">
+      <c r="B140" t="s">
+        <v>12</v>
+      </c>
+      <c r="C140" s="5">
+        <v>40962</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A142" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B140" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A142" s="1" t="s">
+      <c r="B142" t="s">
+        <v>12</v>
+      </c>
+      <c r="C142" s="5">
+        <v>40962</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A144" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B142" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A144" s="1" t="s">
+      <c r="B144" t="s">
+        <v>12</v>
+      </c>
+      <c r="C144" s="5">
+        <v>40962</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A146" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B144" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A146" s="1" t="s">
+      <c r="B146" t="s">
+        <v>12</v>
+      </c>
+      <c r="C146" s="5">
+        <v>40962</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A148" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B146" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A148" s="1" t="s">
+      <c r="B148" t="s">
+        <v>12</v>
+      </c>
+      <c r="C148" s="5">
+        <v>40962</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A150" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B148" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A150" s="1" t="s">
+      <c r="B150" t="s">
+        <v>12</v>
+      </c>
+      <c r="C150" s="5">
+        <v>40962</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A152" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B150" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A152" s="1" t="s">
+      <c r="B152" t="s">
+        <v>12</v>
+      </c>
+      <c r="C152" s="5">
+        <v>40962</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A154" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B152" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A154" s="1" t="s">
+      <c r="B154" t="s">
+        <v>12</v>
+      </c>
+      <c r="C154" s="5">
+        <v>40962</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A156" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B154" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A156" s="1" t="s">
+      <c r="B156" t="s">
+        <v>12</v>
+      </c>
+      <c r="C156" s="5">
+        <v>40962</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A158" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B156" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A158" s="1" t="s">
+      <c r="B158" t="s">
+        <v>12</v>
+      </c>
+      <c r="C158" s="5">
+        <v>40962</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A160" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="B158" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A160" s="1" t="s">
-        <v>100</v>
       </c>
       <c r="B160" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C160" s="5">
+        <v>40962</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B162" t="s">
+        <v>12</v>
+      </c>
+      <c r="C162" s="5">
+        <v>40962</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A164" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B162" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A164" s="1" t="s">
+      <c r="B164" t="s">
+        <v>12</v>
+      </c>
+      <c r="C164" s="5">
+        <v>40962</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A166" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B164" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A166" s="1" t="s">
+      <c r="B166" t="s">
+        <v>12</v>
+      </c>
+      <c r="C166" s="5">
+        <v>40962</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A168" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B166" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A168" s="1" t="s">
+      <c r="B168" t="s">
+        <v>12</v>
+      </c>
+      <c r="C168" s="5">
+        <v>40962</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A170" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B168" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A170" s="1" t="s">
+      <c r="B170" t="s">
+        <v>12</v>
+      </c>
+      <c r="C170" s="5">
+        <v>40962</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A172" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B170" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A172" s="1" t="s">
+      <c r="B172" t="s">
+        <v>12</v>
+      </c>
+      <c r="C172" s="5">
+        <v>40963</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A174" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B172" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A174" s="1" t="s">
+      <c r="B174" t="s">
+        <v>12</v>
+      </c>
+      <c r="C174" s="5">
+        <v>40963</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A176" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B174" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A176" s="1" t="s">
+      <c r="B176" t="s">
+        <v>12</v>
+      </c>
+      <c r="C176" s="5">
+        <v>40963</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A178" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B176" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A178" s="1" t="s">
+      <c r="B178" t="s">
+        <v>12</v>
+      </c>
+      <c r="C178" s="5">
+        <v>40963</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A180" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B178" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A180" s="1" t="s">
+      <c r="B180" t="s">
+        <v>12</v>
+      </c>
+      <c r="C180" s="5">
+        <v>40963</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A182" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B180" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A182" s="1" t="s">
+      <c r="B182" t="s">
+        <v>12</v>
+      </c>
+      <c r="C182" s="5">
+        <v>40963</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A184" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B182" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A184" s="1" t="s">
+      <c r="B184" t="s">
+        <v>12</v>
+      </c>
+      <c r="C184" s="5">
+        <v>40963</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A186" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B184" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A186" s="1" t="s">
+      <c r="B186" t="s">
+        <v>12</v>
+      </c>
+      <c r="C186" s="5">
+        <v>40963</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A188" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B186" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A188" s="1" t="s">
+      <c r="B188" t="s">
+        <v>12</v>
+      </c>
+      <c r="C188" s="5">
+        <v>40963</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A190" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B188" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A190" s="1" t="s">
+      <c r="B190" t="s">
+        <v>12</v>
+      </c>
+      <c r="C190" s="5">
+        <v>40963</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A192" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="B190" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A192" s="1" t="s">
-        <v>116</v>
       </c>
       <c r="B192" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C192" s="5">
+        <v>40963</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B194" t="s">
         <v>117</v>
       </c>
-      <c r="B194" t="s">
+      <c r="C194" s="5">
+        <v>40963</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A196" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A196" s="1" t="s">
+      <c r="B196" t="s">
+        <v>12</v>
+      </c>
+      <c r="C196" s="5">
+        <v>40963</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A198" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B196" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A198" s="1" t="s">
+      <c r="B198" t="s">
+        <v>12</v>
+      </c>
+      <c r="C198" s="5">
+        <v>40963</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A200" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B198" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A200" s="1" t="s">
+      <c r="B200" t="s">
+        <v>12</v>
+      </c>
+      <c r="C200" s="5">
+        <v>40963</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A202" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B200" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A202" s="1" t="s">
+      <c r="B202" t="s">
+        <v>12</v>
+      </c>
+      <c r="C202" s="5">
+        <v>40963</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A204" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B202" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A204" s="1" t="s">
+      <c r="B204" t="s">
+        <v>12</v>
+      </c>
+      <c r="C204" s="5">
+        <v>40963</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A206" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B204" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A206" s="1" t="s">
+      <c r="B206" t="s">
+        <v>12</v>
+      </c>
+      <c r="C206" s="5">
+        <v>40963</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A208" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B206" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A208" s="1" t="s">
+      <c r="B208" t="s">
+        <v>12</v>
+      </c>
+      <c r="C208" s="5">
+        <v>40963</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A210" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B208" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A210" s="1" t="s">
+      <c r="B210" t="s">
+        <v>12</v>
+      </c>
+      <c r="C210" s="5">
+        <v>40964</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A212" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B210" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A212" s="1" t="s">
+      <c r="B212" t="s">
+        <v>12</v>
+      </c>
+      <c r="C212" s="5">
+        <v>40964</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A214" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B212" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A214" s="3" t="s">
+      <c r="B214" t="s">
+        <v>12</v>
+      </c>
+      <c r="C214" s="5">
+        <v>40964</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A216" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B214" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A216" s="1" t="s">
+      <c r="B216" t="s">
+        <v>12</v>
+      </c>
+      <c r="C216" s="5">
+        <v>40964</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A218" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B216" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A218" s="1" t="s">
+      <c r="B218" t="s">
+        <v>12</v>
+      </c>
+      <c r="C218" s="5">
+        <v>40964</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A220" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B218" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A220" s="1" t="s">
+      <c r="B220" t="s">
+        <v>12</v>
+      </c>
+      <c r="C220" s="5">
+        <v>40964</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A222" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B220" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A222" s="1" t="s">
+      <c r="B222" t="s">
+        <v>12</v>
+      </c>
+      <c r="C222" s="5">
+        <v>40964</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A224" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B222" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A224" s="1" t="s">
+      <c r="B224" t="s">
+        <v>12</v>
+      </c>
+      <c r="C224" s="5">
+        <v>40964</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A226" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B224" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A226" s="1" t="s">
+      <c r="B226" t="s">
+        <v>12</v>
+      </c>
+      <c r="C226" s="5">
+        <v>40964</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A228" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B226" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A228" s="1" t="s">
+      <c r="B228" t="s">
+        <v>12</v>
+      </c>
+      <c r="C228" s="5">
+        <v>40964</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A230" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B228" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A230" s="1" t="s">
+      <c r="B230" t="s">
+        <v>12</v>
+      </c>
+      <c r="C230" s="5">
+        <v>40964</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A232" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B230" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A232" s="1" t="s">
+      <c r="B232" t="s">
+        <v>12</v>
+      </c>
+      <c r="C232" s="5">
+        <v>40964</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A234" s="1" t="s">
         <v>137</v>
       </c>
+      <c r="C234" s="5">
+        <v>40965</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A236" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C236" s="5">
+        <v>40965</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A238" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C238" s="5">
+        <v>40965</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A240" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C240" s="5">
+        <v>40965</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A242" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C242" s="5">
+        <v>40965</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A244" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C244" s="5">
+        <v>40965</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A246" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C246" s="5">
+        <v>40965</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A248" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C248" s="5">
+        <v>40965</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A250" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C250" s="5">
+        <v>40965</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A252" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C252" s="5">
+        <v>40965</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A254" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C254" s="5">
+        <v>40965</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A256" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C256" s="5">
+        <v>40965</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A258" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C258" s="5">
+        <v>40965</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A260" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C260" s="5">
+        <v>40965</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A262" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C262" s="5">
+        <v>40965</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A264" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C264" s="5">
+        <v>40965</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A266" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C266" s="5">
+        <v>40965</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A268" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C268" s="5">
+        <v>40965</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A270" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C270" s="5">
+        <v>40965</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A272" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C272" s="5">
+        <v>40965</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A274" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C274" s="5">
+        <v>40965</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A276" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C276" s="5">
+        <v>40965</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A278" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C278" s="5">
+        <v>40965</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C280" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
new history allows castles
</commit_message>
<xml_diff>
--- a/ActionPlan.xlsx
+++ b/ActionPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leo\Personal\Projects\lila\li-ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92E42B0-36D0-4ECA-BEC3-C99A30691173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74EEEBE4-D419-4599-BF85-1F977B3D7FC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1C291D5E-1E99-48BC-A46C-6EAD5B360DBF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="160">
   <si>
     <t>.gitignore</t>
   </si>
@@ -894,8 +894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E2963DC-9FBA-42E8-B13F-F42B9BDE156E}">
   <dimension ref="A1:E280"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A228" workbookViewId="0">
-      <selection activeCell="C236" sqref="C236"/>
+    <sheetView tabSelected="1" topLeftCell="A231" workbookViewId="0">
+      <selection activeCell="C238" sqref="C238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2314,6 +2314,9 @@
       <c r="A238" s="1" t="s">
         <v>139</v>
       </c>
+      <c r="B238" t="s">
+        <v>12</v>
+      </c>
       <c r="C238" s="5">
         <v>40965</v>
       </c>

</xml_diff>

<commit_message>
rook moves prevent castling
</commit_message>
<xml_diff>
--- a/ActionPlan.xlsx
+++ b/ActionPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leo\Personal\Projects\lila\li-ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{723AF707-6A73-4545-A0D7-1F811F55B1E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CCB81CA-43E0-4A2E-86D7-70548DC5EF36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1C291D5E-1E99-48BC-A46C-6EAD5B360DBF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="160">
   <si>
     <t>.gitignore</t>
   </si>
@@ -895,7 +895,7 @@
   <dimension ref="A1:E280"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A231" workbookViewId="0">
-      <selection activeCell="C240" sqref="C240"/>
+      <selection activeCell="C242" sqref="C242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2336,6 +2336,9 @@
       <c r="A242" s="1" t="s">
         <v>141</v>
       </c>
+      <c r="B242" t="s">
+        <v>12</v>
+      </c>
       <c r="C242" s="5">
         <v>40965</v>
       </c>

</xml_diff>

<commit_message>
moving king prevents castling
</commit_message>
<xml_diff>
--- a/ActionPlan.xlsx
+++ b/ActionPlan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leo\Personal\Projects\lila\li-ja\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leo\Projects\lila\li-ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CCB81CA-43E0-4A2E-86D7-70548DC5EF36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D21B90CE-0941-4757-98DE-63E4E045692D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1C291D5E-1E99-48BC-A46C-6EAD5B360DBF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1C291D5E-1E99-48BC-A46C-6EAD5B360DBF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="160">
   <si>
     <t>.gitignore</t>
   </si>
@@ -895,16 +895,16 @@
   <dimension ref="A1:E280"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A231" workbookViewId="0">
-      <selection activeCell="C242" sqref="C242"/>
+      <selection activeCell="C244" sqref="C244"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -916,7 +916,7 @@
         <v xml:space="preserve"> installation</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -924,7 +924,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -932,7 +932,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -940,7 +940,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -948,7 +948,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -956,7 +956,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -964,7 +964,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -972,7 +972,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -980,7 +980,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -988,7 +988,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -996,7 +996,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>40958</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -1020,7 +1020,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1036,7 +1036,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1060,7 +1060,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -1068,7 +1068,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>33</v>
       </c>
@@ -1076,12 +1076,12 @@
         <v>40960</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>21</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -1108,7 +1108,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>23</v>
       </c>
@@ -1119,7 +1119,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -1130,7 +1130,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>24</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>25</v>
       </c>
@@ -1149,7 +1149,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>26</v>
       </c>
@@ -1157,7 +1157,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>18</v>
       </c>
@@ -1168,7 +1168,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>27</v>
       </c>
@@ -1176,7 +1176,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>7</v>
       </c>
@@ -1184,7 +1184,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>34</v>
       </c>
@@ -1192,7 +1192,7 @@
         <v>40960</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>35</v>
       </c>
@@ -1200,7 +1200,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>36</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>40960</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>17</v>
       </c>
@@ -1216,7 +1216,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>19</v>
       </c>
@@ -1224,7 +1224,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>37</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>38</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>40960</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>23</v>
       </c>
@@ -1248,7 +1248,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>24</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>26</v>
       </c>
@@ -1264,7 +1264,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>39</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>40960</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>23</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>40</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>40960</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>41</v>
       </c>
@@ -1302,7 +1302,7 @@
         <v>40960</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>42</v>
       </c>
@@ -1313,7 +1313,7 @@
         <v>40960</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>43</v>
       </c>
@@ -1324,7 +1324,7 @@
         <v>40960</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>44</v>
       </c>
@@ -1335,7 +1335,7 @@
         <v>40960</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>45</v>
       </c>
@@ -1346,7 +1346,7 @@
         <v>40960</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>46</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>40960</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>47</v>
       </c>
@@ -1368,7 +1368,7 @@
         <v>40960</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>48</v>
       </c>
@@ -1376,7 +1376,7 @@
         <v>40960</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>21</v>
       </c>
@@ -1384,7 +1384,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>22</v>
       </c>
@@ -1392,7 +1392,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>23</v>
       </c>
@@ -1400,7 +1400,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>24</v>
       </c>
@@ -1408,7 +1408,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>49</v>
       </c>
@@ -1416,7 +1416,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>27</v>
       </c>
@@ -1424,7 +1424,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>50</v>
       </c>
@@ -1432,7 +1432,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>51</v>
       </c>
@@ -1443,7 +1443,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>52</v>
       </c>
@@ -1454,7 +1454,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>53</v>
       </c>
@@ -1465,7 +1465,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>54</v>
       </c>
@@ -1473,7 +1473,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>55</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>56</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>57</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>58</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>59</v>
       </c>
@@ -1513,7 +1513,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>60</v>
       </c>
@@ -1521,7 +1521,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>61</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>63</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>7</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>64</v>
       </c>
@@ -1556,7 +1556,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>65</v>
       </c>
@@ -1564,7 +1564,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>66</v>
       </c>
@@ -1572,7 +1572,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>67</v>
       </c>
@@ -1580,7 +1580,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>58</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>68</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>69</v>
       </c>
@@ -1604,7 +1604,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>60</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>70</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>71</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>75</v>
       </c>
@@ -1639,7 +1639,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>76</v>
       </c>
@@ -1650,7 +1650,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>77</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>78</v>
       </c>
@@ -1672,7 +1672,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>80</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>81</v>
       </c>
@@ -1694,7 +1694,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>82</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>83</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>84</v>
       </c>
@@ -1727,7 +1727,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>85</v>
       </c>
@@ -1738,7 +1738,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>86</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>87</v>
       </c>
@@ -1760,7 +1760,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>88</v>
       </c>
@@ -1771,7 +1771,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>89</v>
       </c>
@@ -1782,7 +1782,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>90</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>91</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>92</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>93</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>94</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>95</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>96</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>97</v>
       </c>
@@ -1870,7 +1870,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>98</v>
       </c>
@@ -1881,7 +1881,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>99</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>100</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>101</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>102</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>103</v>
       </c>
@@ -1936,7 +1936,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>104</v>
       </c>
@@ -1947,7 +1947,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>105</v>
       </c>
@@ -1958,7 +1958,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>106</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>107</v>
       </c>
@@ -1980,7 +1980,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>108</v>
       </c>
@@ -1991,7 +1991,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>109</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>110</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>111</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>112</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>113</v>
       </c>
@@ -2046,7 +2046,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>114</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>115</v>
       </c>
@@ -2068,7 +2068,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>116</v>
       </c>
@@ -2079,7 +2079,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>118</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>119</v>
       </c>
@@ -2101,7 +2101,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>120</v>
       </c>
@@ -2112,7 +2112,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
         <v>121</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>122</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
         <v>123</v>
       </c>
@@ -2145,7 +2145,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
         <v>124</v>
       </c>
@@ -2156,7 +2156,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
         <v>125</v>
       </c>
@@ -2167,7 +2167,7 @@
         <v>40964</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>126</v>
       </c>
@@ -2178,7 +2178,7 @@
         <v>40964</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" s="3" t="s">
         <v>127</v>
       </c>
@@ -2189,7 +2189,7 @@
         <v>40964</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
         <v>128</v>
       </c>
@@ -2200,7 +2200,7 @@
         <v>40964</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>129</v>
       </c>
@@ -2211,7 +2211,7 @@
         <v>40964</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
         <v>130</v>
       </c>
@@ -2222,7 +2222,7 @@
         <v>40964</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
         <v>131</v>
       </c>
@@ -2233,7 +2233,7 @@
         <v>40964</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
         <v>132</v>
       </c>
@@ -2244,7 +2244,7 @@
         <v>40964</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>133</v>
       </c>
@@ -2255,7 +2255,7 @@
         <v>40964</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
         <v>134</v>
       </c>
@@ -2266,7 +2266,7 @@
         <v>40964</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
         <v>135</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>40964</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
         <v>136</v>
       </c>
@@ -2288,7 +2288,7 @@
         <v>40964</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
         <v>137</v>
       </c>
@@ -2299,7 +2299,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
         <v>138</v>
       </c>
@@ -2310,7 +2310,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
         <v>139</v>
       </c>
@@ -2321,7 +2321,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
         <v>140</v>
       </c>
@@ -2332,7 +2332,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
         <v>141</v>
       </c>
@@ -2343,15 +2343,18 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
         <v>142</v>
       </c>
+      <c r="B244" t="s">
+        <v>12</v>
+      </c>
       <c r="C244" s="5">
         <v>40965</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
         <v>143</v>
       </c>
@@ -2359,7 +2362,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
         <v>144</v>
       </c>
@@ -2367,7 +2370,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
         <v>145</v>
       </c>
@@ -2375,7 +2378,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
         <v>146</v>
       </c>
@@ -2383,7 +2386,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
         <v>147</v>
       </c>
@@ -2391,7 +2394,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
         <v>148</v>
       </c>
@@ -2399,7 +2402,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
         <v>149</v>
       </c>
@@ -2407,7 +2410,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
         <v>150</v>
       </c>
@@ -2415,7 +2418,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
         <v>151</v>
       </c>
@@ -2423,7 +2426,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
         <v>152</v>
       </c>
@@ -2431,7 +2434,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
         <v>153</v>
       </c>
@@ -2439,7 +2442,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
         <v>154</v>
       </c>
@@ -2447,7 +2450,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
         <v>155</v>
       </c>
@@ -2455,7 +2458,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
         <v>156</v>
       </c>
@@ -2463,7 +2466,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
         <v>157</v>
       </c>
@@ -2471,7 +2474,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
         <v>158</v>
       </c>
@@ -2479,7 +2482,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
         <v>159</v>
       </c>
@@ -2487,7 +2490,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C280" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
castle under threat tests
</commit_message>
<xml_diff>
--- a/ActionPlan.xlsx
+++ b/ActionPlan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leo\Projects\lila\li-ja\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leo\Personal\Projects\lila\li-ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FF023A2-18B3-4EC7-824E-145D9FD22818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C68A68C-A14D-46AE-BFE8-EF6D76A406F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1C291D5E-1E99-48BC-A46C-6EAD5B360DBF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1C291D5E-1E99-48BC-A46C-6EAD5B360DBF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="160">
   <si>
     <t>.gitignore</t>
   </si>
@@ -894,17 +894,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E2963DC-9FBA-42E8-B13F-F42B9BDE156E}">
   <dimension ref="A1:E280"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A231" workbookViewId="0">
-      <selection activeCell="C246" sqref="C246"/>
+    <sheetView tabSelected="1" topLeftCell="A238" workbookViewId="0">
+      <selection activeCell="C248" sqref="C248"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="55.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -916,7 +916,7 @@
         <v xml:space="preserve"> installation</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -924,7 +924,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -932,7 +932,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -940,7 +940,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -948,7 +948,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -956,7 +956,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -964,7 +964,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -972,7 +972,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -980,7 +980,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -988,7 +988,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -996,7 +996,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>40958</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -1020,7 +1020,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1036,7 +1036,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1060,7 +1060,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -1068,7 +1068,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>33</v>
       </c>
@@ -1076,12 +1076,12 @@
         <v>40960</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>21</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -1108,7 +1108,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>23</v>
       </c>
@@ -1119,7 +1119,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -1130,7 +1130,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>24</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>25</v>
       </c>
@@ -1149,7 +1149,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>26</v>
       </c>
@@ -1157,7 +1157,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>18</v>
       </c>
@@ -1168,7 +1168,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>27</v>
       </c>
@@ -1176,7 +1176,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>7</v>
       </c>
@@ -1184,7 +1184,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>34</v>
       </c>
@@ -1192,7 +1192,7 @@
         <v>40960</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>35</v>
       </c>
@@ -1200,7 +1200,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>36</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>40960</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>17</v>
       </c>
@@ -1216,7 +1216,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>19</v>
       </c>
@@ -1224,7 +1224,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>37</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>38</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>40960</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>23</v>
       </c>
@@ -1248,7 +1248,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>24</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>26</v>
       </c>
@@ -1264,7 +1264,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>39</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>40960</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>23</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>40</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>40960</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>41</v>
       </c>
@@ -1302,7 +1302,7 @@
         <v>40960</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>42</v>
       </c>
@@ -1313,7 +1313,7 @@
         <v>40960</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
         <v>43</v>
       </c>
@@ -1324,7 +1324,7 @@
         <v>40960</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>44</v>
       </c>
@@ -1335,7 +1335,7 @@
         <v>40960</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>45</v>
       </c>
@@ -1346,7 +1346,7 @@
         <v>40960</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>46</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>40960</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>47</v>
       </c>
@@ -1368,7 +1368,7 @@
         <v>40960</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>48</v>
       </c>
@@ -1376,7 +1376,7 @@
         <v>40960</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>21</v>
       </c>
@@ -1384,7 +1384,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>22</v>
       </c>
@@ -1392,7 +1392,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>23</v>
       </c>
@@ -1400,7 +1400,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>24</v>
       </c>
@@ -1408,7 +1408,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>49</v>
       </c>
@@ -1416,7 +1416,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>27</v>
       </c>
@@ -1424,7 +1424,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>50</v>
       </c>
@@ -1432,7 +1432,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>51</v>
       </c>
@@ -1443,7 +1443,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
         <v>52</v>
       </c>
@@ -1454,7 +1454,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>53</v>
       </c>
@@ -1465,7 +1465,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>54</v>
       </c>
@@ -1473,7 +1473,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>55</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>56</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>57</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>58</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>59</v>
       </c>
@@ -1513,7 +1513,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>60</v>
       </c>
@@ -1521,7 +1521,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>61</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>63</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>7</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>64</v>
       </c>
@@ -1556,7 +1556,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>65</v>
       </c>
@@ -1564,7 +1564,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>66</v>
       </c>
@@ -1572,7 +1572,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>67</v>
       </c>
@@ -1580,7 +1580,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>58</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>68</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>69</v>
       </c>
@@ -1604,7 +1604,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>60</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>70</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>71</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>75</v>
       </c>
@@ -1639,7 +1639,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>76</v>
       </c>
@@ -1650,7 +1650,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>77</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>78</v>
       </c>
@@ -1672,7 +1672,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>80</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>81</v>
       </c>
@@ -1694,7 +1694,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>82</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>83</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>84</v>
       </c>
@@ -1727,7 +1727,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
         <v>85</v>
       </c>
@@ -1738,7 +1738,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
         <v>86</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
         <v>87</v>
       </c>
@@ -1760,7 +1760,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
         <v>88</v>
       </c>
@@ -1771,7 +1771,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
         <v>89</v>
       </c>
@@ -1782,7 +1782,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
         <v>90</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
         <v>91</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
         <v>92</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
         <v>93</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
         <v>94</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
         <v>95</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
         <v>96</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
         <v>97</v>
       </c>
@@ -1870,7 +1870,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
         <v>98</v>
       </c>
@@ -1881,7 +1881,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
         <v>99</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
         <v>100</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="s">
         <v>101</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="s">
         <v>102</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
         <v>103</v>
       </c>
@@ -1936,7 +1936,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" s="1" t="s">
         <v>104</v>
       </c>
@@ -1947,7 +1947,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" s="1" t="s">
         <v>105</v>
       </c>
@@ -1958,7 +1958,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" s="1" t="s">
         <v>106</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" s="1" t="s">
         <v>107</v>
       </c>
@@ -1980,7 +1980,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" s="1" t="s">
         <v>108</v>
       </c>
@@ -1991,7 +1991,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180" s="1" t="s">
         <v>109</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182" s="1" t="s">
         <v>110</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
         <v>111</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A186" s="1" t="s">
         <v>112</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A188" s="1" t="s">
         <v>113</v>
       </c>
@@ -2046,7 +2046,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A190" s="1" t="s">
         <v>114</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A192" s="1" t="s">
         <v>115</v>
       </c>
@@ -2068,7 +2068,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194" s="1" t="s">
         <v>116</v>
       </c>
@@ -2079,7 +2079,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196" s="1" t="s">
         <v>118</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A198" s="1" t="s">
         <v>119</v>
       </c>
@@ -2101,7 +2101,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A200" s="1" t="s">
         <v>120</v>
       </c>
@@ -2112,7 +2112,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A202" s="1" t="s">
         <v>121</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A204" s="1" t="s">
         <v>122</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A206" s="1" t="s">
         <v>123</v>
       </c>
@@ -2145,7 +2145,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A208" s="1" t="s">
         <v>124</v>
       </c>
@@ -2156,7 +2156,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A210" s="1" t="s">
         <v>125</v>
       </c>
@@ -2167,7 +2167,7 @@
         <v>40964</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A212" s="1" t="s">
         <v>126</v>
       </c>
@@ -2178,7 +2178,7 @@
         <v>40964</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A214" s="3" t="s">
         <v>127</v>
       </c>
@@ -2189,7 +2189,7 @@
         <v>40964</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A216" s="1" t="s">
         <v>128</v>
       </c>
@@ -2200,7 +2200,7 @@
         <v>40964</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A218" s="1" t="s">
         <v>129</v>
       </c>
@@ -2211,7 +2211,7 @@
         <v>40964</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A220" s="1" t="s">
         <v>130</v>
       </c>
@@ -2222,7 +2222,7 @@
         <v>40964</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A222" s="1" t="s">
         <v>131</v>
       </c>
@@ -2233,7 +2233,7 @@
         <v>40964</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A224" s="1" t="s">
         <v>132</v>
       </c>
@@ -2244,7 +2244,7 @@
         <v>40964</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A226" s="1" t="s">
         <v>133</v>
       </c>
@@ -2255,7 +2255,7 @@
         <v>40964</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A228" s="1" t="s">
         <v>134</v>
       </c>
@@ -2266,7 +2266,7 @@
         <v>40964</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A230" s="1" t="s">
         <v>135</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>40964</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A232" s="1" t="s">
         <v>136</v>
       </c>
@@ -2288,7 +2288,7 @@
         <v>40964</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A234" s="1" t="s">
         <v>137</v>
       </c>
@@ -2299,7 +2299,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A236" s="1" t="s">
         <v>138</v>
       </c>
@@ -2310,7 +2310,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A238" s="1" t="s">
         <v>139</v>
       </c>
@@ -2321,7 +2321,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A240" s="1" t="s">
         <v>140</v>
       </c>
@@ -2332,7 +2332,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A242" s="1" t="s">
         <v>141</v>
       </c>
@@ -2343,7 +2343,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A244" s="1" t="s">
         <v>142</v>
       </c>
@@ -2354,7 +2354,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A246" s="1" t="s">
         <v>143</v>
       </c>
@@ -2365,15 +2365,18 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A248" s="1" t="s">
         <v>144</v>
       </c>
+      <c r="B248" t="s">
+        <v>12</v>
+      </c>
       <c r="C248" s="5">
         <v>40965</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A250" s="1" t="s">
         <v>145</v>
       </c>
@@ -2381,7 +2384,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A252" s="1" t="s">
         <v>146</v>
       </c>
@@ -2389,7 +2392,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A254" s="1" t="s">
         <v>147</v>
       </c>
@@ -2397,7 +2400,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A256" s="1" t="s">
         <v>148</v>
       </c>
@@ -2405,7 +2408,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A258" s="1" t="s">
         <v>149</v>
       </c>
@@ -2413,7 +2416,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A260" s="1" t="s">
         <v>150</v>
       </c>
@@ -2421,7 +2424,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A262" s="1" t="s">
         <v>151</v>
       </c>
@@ -2429,7 +2432,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A264" s="1" t="s">
         <v>152</v>
       </c>
@@ -2437,7 +2440,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A266" s="1" t="s">
         <v>153</v>
       </c>
@@ -2445,7 +2448,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A268" s="1" t="s">
         <v>154</v>
       </c>
@@ -2453,7 +2456,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A270" s="1" t="s">
         <v>155</v>
       </c>
@@ -2461,7 +2464,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A272" s="1" t="s">
         <v>156</v>
       </c>
@@ -2469,7 +2472,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A274" s="1" t="s">
         <v>157</v>
       </c>
@@ -2477,7 +2480,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A276" s="1" t="s">
         <v>158</v>
       </c>
@@ -2485,7 +2488,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A278" s="1" t="s">
         <v>159</v>
       </c>
@@ -2493,7 +2496,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C280" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Don't castle if the enemy threatens part of the king trip
</commit_message>
<xml_diff>
--- a/ActionPlan.xlsx
+++ b/ActionPlan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leo\Personal\Projects\lila\li-ja\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leo\Projects\lila\li-ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C68A68C-A14D-46AE-BFE8-EF6D76A406F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D936078-CDDD-4262-8153-016046C9F9ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1C291D5E-1E99-48BC-A46C-6EAD5B360DBF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1C291D5E-1E99-48BC-A46C-6EAD5B360DBF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="160">
   <si>
     <t>.gitignore</t>
   </si>
@@ -895,16 +895,16 @@
   <dimension ref="A1:E280"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A238" workbookViewId="0">
-      <selection activeCell="C248" sqref="C248"/>
+      <selection activeCell="C250" sqref="C250"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -916,7 +916,7 @@
         <v xml:space="preserve"> installation</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -924,7 +924,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -932,7 +932,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -940,7 +940,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -948,7 +948,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -956,7 +956,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -964,7 +964,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -972,7 +972,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -980,7 +980,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -988,7 +988,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -996,7 +996,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>40958</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -1020,7 +1020,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1036,7 +1036,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1060,7 +1060,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -1068,7 +1068,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>33</v>
       </c>
@@ -1076,12 +1076,12 @@
         <v>40960</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>21</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -1108,7 +1108,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>23</v>
       </c>
@@ -1119,7 +1119,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -1130,7 +1130,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>24</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>25</v>
       </c>
@@ -1149,7 +1149,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>26</v>
       </c>
@@ -1157,7 +1157,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>18</v>
       </c>
@@ -1168,7 +1168,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>27</v>
       </c>
@@ -1176,7 +1176,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>7</v>
       </c>
@@ -1184,7 +1184,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>34</v>
       </c>
@@ -1192,7 +1192,7 @@
         <v>40960</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>35</v>
       </c>
@@ -1200,7 +1200,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>36</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>40960</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>17</v>
       </c>
@@ -1216,7 +1216,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>19</v>
       </c>
@@ -1224,7 +1224,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>37</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>38</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>40960</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>23</v>
       </c>
@@ -1248,7 +1248,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>24</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>26</v>
       </c>
@@ -1264,7 +1264,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>39</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>40960</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>23</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>40</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>40960</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>41</v>
       </c>
@@ -1302,7 +1302,7 @@
         <v>40960</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>42</v>
       </c>
@@ -1313,7 +1313,7 @@
         <v>40960</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>43</v>
       </c>
@@ -1324,7 +1324,7 @@
         <v>40960</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>44</v>
       </c>
@@ -1335,7 +1335,7 @@
         <v>40960</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>45</v>
       </c>
@@ -1346,7 +1346,7 @@
         <v>40960</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>46</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>40960</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>47</v>
       </c>
@@ -1368,7 +1368,7 @@
         <v>40960</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>48</v>
       </c>
@@ -1376,7 +1376,7 @@
         <v>40960</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>21</v>
       </c>
@@ -1384,7 +1384,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>22</v>
       </c>
@@ -1392,7 +1392,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>23</v>
       </c>
@@ -1400,7 +1400,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>24</v>
       </c>
@@ -1408,7 +1408,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>49</v>
       </c>
@@ -1416,7 +1416,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>27</v>
       </c>
@@ -1424,7 +1424,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>50</v>
       </c>
@@ -1432,7 +1432,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>51</v>
       </c>
@@ -1443,7 +1443,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>52</v>
       </c>
@@ -1454,7 +1454,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>53</v>
       </c>
@@ -1465,7 +1465,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>54</v>
       </c>
@@ -1473,7 +1473,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>55</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>56</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>57</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>58</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>59</v>
       </c>
@@ -1513,7 +1513,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>60</v>
       </c>
@@ -1521,7 +1521,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>61</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>63</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>7</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>64</v>
       </c>
@@ -1556,7 +1556,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>65</v>
       </c>
@@ -1564,7 +1564,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>66</v>
       </c>
@@ -1572,7 +1572,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>67</v>
       </c>
@@ -1580,7 +1580,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>58</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>68</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>69</v>
       </c>
@@ -1604,7 +1604,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>60</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>70</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>71</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>75</v>
       </c>
@@ -1639,7 +1639,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>76</v>
       </c>
@@ -1650,7 +1650,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>77</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>78</v>
       </c>
@@ -1672,7 +1672,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>80</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>81</v>
       </c>
@@ -1694,7 +1694,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>82</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>83</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>84</v>
       </c>
@@ -1727,7 +1727,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>85</v>
       </c>
@@ -1738,7 +1738,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>86</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>87</v>
       </c>
@@ -1760,7 +1760,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>88</v>
       </c>
@@ -1771,7 +1771,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>89</v>
       </c>
@@ -1782,7 +1782,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>90</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>91</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>92</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>93</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>94</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>95</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>96</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>97</v>
       </c>
@@ -1870,7 +1870,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>98</v>
       </c>
@@ -1881,7 +1881,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>99</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>100</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>101</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>102</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>103</v>
       </c>
@@ -1936,7 +1936,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>104</v>
       </c>
@@ -1947,7 +1947,7 @@
         <v>40962</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>105</v>
       </c>
@@ -1958,7 +1958,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>106</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>107</v>
       </c>
@@ -1980,7 +1980,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>108</v>
       </c>
@@ -1991,7 +1991,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>109</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>110</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>111</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>112</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>113</v>
       </c>
@@ -2046,7 +2046,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>114</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>115</v>
       </c>
@@ -2068,7 +2068,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>116</v>
       </c>
@@ -2079,7 +2079,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>118</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>119</v>
       </c>
@@ -2101,7 +2101,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>120</v>
       </c>
@@ -2112,7 +2112,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
         <v>121</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>122</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
         <v>123</v>
       </c>
@@ -2145,7 +2145,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
         <v>124</v>
       </c>
@@ -2156,7 +2156,7 @@
         <v>40963</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
         <v>125</v>
       </c>
@@ -2167,7 +2167,7 @@
         <v>40964</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>126</v>
       </c>
@@ -2178,7 +2178,7 @@
         <v>40964</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" s="3" t="s">
         <v>127</v>
       </c>
@@ -2189,7 +2189,7 @@
         <v>40964</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
         <v>128</v>
       </c>
@@ -2200,7 +2200,7 @@
         <v>40964</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>129</v>
       </c>
@@ -2211,7 +2211,7 @@
         <v>40964</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
         <v>130</v>
       </c>
@@ -2222,7 +2222,7 @@
         <v>40964</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
         <v>131</v>
       </c>
@@ -2233,7 +2233,7 @@
         <v>40964</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
         <v>132</v>
       </c>
@@ -2244,7 +2244,7 @@
         <v>40964</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>133</v>
       </c>
@@ -2255,7 +2255,7 @@
         <v>40964</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
         <v>134</v>
       </c>
@@ -2266,7 +2266,7 @@
         <v>40964</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
         <v>135</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>40964</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
         <v>136</v>
       </c>
@@ -2288,7 +2288,7 @@
         <v>40964</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
         <v>137</v>
       </c>
@@ -2299,7 +2299,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
         <v>138</v>
       </c>
@@ -2310,7 +2310,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
         <v>139</v>
       </c>
@@ -2321,7 +2321,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
         <v>140</v>
       </c>
@@ -2332,7 +2332,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
         <v>141</v>
       </c>
@@ -2343,7 +2343,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
         <v>142</v>
       </c>
@@ -2354,7 +2354,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
         <v>143</v>
       </c>
@@ -2365,7 +2365,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
         <v>144</v>
       </c>
@@ -2376,15 +2376,18 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
         <v>145</v>
       </c>
+      <c r="B250" t="s">
+        <v>12</v>
+      </c>
       <c r="C250" s="5">
         <v>40965</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
         <v>146</v>
       </c>
@@ -2392,7 +2395,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
         <v>147</v>
       </c>
@@ -2400,7 +2403,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
         <v>148</v>
       </c>
@@ -2408,7 +2411,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
         <v>149</v>
       </c>
@@ -2416,7 +2419,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
         <v>150</v>
       </c>
@@ -2424,7 +2427,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
         <v>151</v>
       </c>
@@ -2432,7 +2435,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
         <v>152</v>
       </c>
@@ -2440,7 +2443,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
         <v>153</v>
       </c>
@@ -2448,7 +2451,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
         <v>154</v>
       </c>
@@ -2456,7 +2459,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
         <v>155</v>
       </c>
@@ -2464,7 +2467,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
         <v>156</v>
       </c>
@@ -2472,7 +2475,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
         <v>157</v>
       </c>
@@ -2480,7 +2483,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
         <v>158</v>
       </c>
@@ -2488,7 +2491,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
         <v>159</v>
       </c>
@@ -2496,7 +2499,7 @@
         <v>40965</v>
       </c>
     </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C280" s="5"/>
     </row>
   </sheetData>

</xml_diff>